<commit_message>
Finished, incl. comments. Aan de noise waardes kan nog getweaked worden
</commit_message>
<xml_diff>
--- a/runway-allocation - Correct/Full_Tables.xlsx
+++ b/runway-allocation - Correct/Full_Tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hofma\Documents\runway-allocation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luka\Documents\runway-allocation\runway-allocation - Correct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D43927-4C1C-43BD-A5B9-164D281F82EB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D46BCCA-02A3-4C73-987A-47B6D0E3AD5C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8496" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="R06_Arr_M" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="29">
   <si>
     <t>Nr</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>All ARTIP</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
   </si>
 </sst>
 </file>
@@ -1596,7 +1602,7 @@
         <v>2</v>
       </c>
       <c r="P3" s="33">
-        <f t="shared" ref="P3:P8" si="0">J3</f>
+        <f t="shared" ref="P3:P7" si="0">J3</f>
         <v>156.80000000000001</v>
       </c>
       <c r="Q3" s="32"/>
@@ -1911,7 +1917,7 @@
         <v>2</v>
       </c>
       <c r="P10" s="33">
-        <f t="shared" ref="P10:P15" si="1">J17</f>
+        <f t="shared" ref="P10:P14" si="1">J17</f>
         <v>273.08000000000004</v>
       </c>
       <c r="Q10" s="32"/>
@@ -2217,7 +2223,7 @@
         <v>2</v>
       </c>
       <c r="P17" s="33">
-        <f t="shared" ref="P17:P22" si="2">J31</f>
+        <f t="shared" ref="P17:P21" si="2">J31</f>
         <v>275.60000000000002</v>
       </c>
       <c r="R17" s="41"/>
@@ -2511,7 +2517,7 @@
         <v>2</v>
       </c>
       <c r="P24" s="33">
-        <f t="shared" ref="P24:P29" si="3">J45</f>
+        <f t="shared" ref="P24:P28" si="3">J45</f>
         <v>123.48</v>
       </c>
       <c r="R24" s="41"/>
@@ -2804,7 +2810,7 @@
         <v>2</v>
       </c>
       <c r="P31" s="33">
-        <f t="shared" ref="P31:P36" si="4">J59</f>
+        <f t="shared" ref="P31:P35" si="4">J59</f>
         <v>410.2</v>
       </c>
     </row>
@@ -3091,7 +3097,7 @@
         <v>2</v>
       </c>
       <c r="P38" s="33">
-        <f t="shared" ref="P38:P43" si="5">J73</f>
+        <f t="shared" ref="P38:P42" si="5">J73</f>
         <v>584.10000000000014</v>
       </c>
     </row>
@@ -3378,7 +3384,7 @@
         <v>2</v>
       </c>
       <c r="P45" s="33">
-        <f t="shared" ref="P45:P50" si="6">J87</f>
+        <f t="shared" ref="P45:P49" si="6">J87</f>
         <v>275.60000000000002</v>
       </c>
     </row>
@@ -3665,7 +3671,7 @@
         <v>2</v>
       </c>
       <c r="P52" s="33">
-        <f t="shared" ref="P52:P57" si="7">J101</f>
+        <f t="shared" ref="P52:P56" si="7">J101</f>
         <v>123.48</v>
       </c>
     </row>
@@ -3952,7 +3958,7 @@
         <v>2</v>
       </c>
       <c r="P59" s="47">
-        <f t="shared" ref="P59:P64" si="8">J115</f>
+        <f t="shared" ref="P59:P63" si="8">J115</f>
         <v>410.2</v>
       </c>
     </row>
@@ -4239,7 +4245,7 @@
         <v>2</v>
       </c>
       <c r="P66" s="47">
-        <f t="shared" ref="P66:P71" si="9">J129</f>
+        <f t="shared" ref="P66:P70" si="9">J129</f>
         <v>584.10000000000014</v>
       </c>
     </row>
@@ -4526,7 +4532,7 @@
         <v>2</v>
       </c>
       <c r="P73" s="47">
-        <f t="shared" ref="P73:P78" si="10">J143</f>
+        <f t="shared" ref="P73:P77" si="10">J143</f>
         <v>156.80000000000001</v>
       </c>
     </row>
@@ -4813,7 +4819,7 @@
         <v>2</v>
       </c>
       <c r="P80" s="47">
-        <f t="shared" ref="P80:P85" si="11">J157</f>
+        <f t="shared" ref="P80:P84" si="11">J157</f>
         <v>273.08000000000004</v>
       </c>
     </row>
@@ -5100,7 +5106,7 @@
         <v>2</v>
       </c>
       <c r="P87" s="47">
-        <f t="shared" ref="P87:P92" si="14">J171</f>
+        <f t="shared" ref="P87:P91" si="14">J171</f>
         <v>664.6</v>
       </c>
     </row>
@@ -5387,7 +5393,7 @@
         <v>2</v>
       </c>
       <c r="P94" s="47">
-        <f t="shared" ref="P94:P99" si="15">J185</f>
+        <f t="shared" ref="P94:P98" si="15">J185</f>
         <v>297.89999999999998</v>
       </c>
     </row>
@@ -5674,7 +5680,7 @@
         <v>2</v>
       </c>
       <c r="P101" s="47">
-        <f t="shared" ref="P101:P106" si="17">J199</f>
+        <f t="shared" ref="P101:P105" si="17">J199</f>
         <v>378.40000000000003</v>
       </c>
     </row>
@@ -5961,7 +5967,7 @@
         <v>2</v>
       </c>
       <c r="P108" s="33">
-        <f t="shared" ref="P108:P113" si="18">J213</f>
+        <f t="shared" ref="P108:P112" si="18">J213</f>
         <v>658.30000000000007</v>
       </c>
     </row>
@@ -6248,7 +6254,7 @@
         <v>2</v>
       </c>
       <c r="P115" s="33">
-        <f t="shared" ref="P115:P120" si="22">J227</f>
+        <f t="shared" ref="P115:P119" si="22">J227</f>
         <v>170</v>
       </c>
     </row>
@@ -6535,7 +6541,7 @@
         <v>2</v>
       </c>
       <c r="P122" s="33">
-        <f t="shared" ref="P122:P127" si="23">J241</f>
+        <f t="shared" ref="P122:P126" si="23">J241</f>
         <v>242.28000000000003</v>
       </c>
     </row>
@@ -6822,7 +6828,7 @@
         <v>2</v>
       </c>
       <c r="P129" s="33">
-        <f t="shared" ref="P129:P134" si="24">J255</f>
+        <f t="shared" ref="P129:P133" si="24">J255</f>
         <v>275.60000000000002</v>
       </c>
     </row>
@@ -7109,7 +7115,7 @@
         <v>2</v>
       </c>
       <c r="P136" s="33">
-        <f t="shared" ref="P136:P141" si="25">J269</f>
+        <f t="shared" ref="P136:P140" si="25">J269</f>
         <v>123.48</v>
       </c>
     </row>
@@ -11247,7 +11253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F2A5A1-E880-4844-A90B-E2D712D9D7B7}">
   <dimension ref="A1:Z281"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
@@ -23956,15 +23962,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD6EA91-B2D9-460A-B72F-58023DD02AD7}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="37" t="s">
         <v>13</v>
       </c>
@@ -23981,7 +23987,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="31">
         <v>220</v>
       </c>
@@ -23995,8 +24001,19 @@
         <f>t_to_RWY!B4</f>
         <v>640</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <f>t_to_RWY!C4</f>
+        <v>1180</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2">
+        <f>MIN(E2:F11)</f>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="31">
         <v>180</v>
       </c>
@@ -24006,12 +24023,27 @@
       <c r="C3" s="33" t="s">
         <v>9</v>
       </c>
+      <c r="D3">
+        <f>$A3</f>
+        <v>180</v>
+      </c>
       <c r="E3">
-        <f>t_to_RWY!B3+A3</f>
+        <f>t_to_RWY!B3+$D3</f>
         <v>1360</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <f>t_to_RWY!C3+$D3</f>
+        <v>680</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3">
+        <f>MAX(E2:F11)</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="31">
         <v>140</v>
       </c>
@@ -24021,12 +24053,20 @@
       <c r="C4" s="33" t="s">
         <v>10</v>
       </c>
+      <c r="D4">
+        <f>$D3+$A4</f>
+        <v>320</v>
+      </c>
       <c r="E4">
-        <f>A3+A4+t_to_RWY!B2</f>
+        <f>$D4+t_to_RWY!B2</f>
         <v>1020</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <f>$D4+t_to_RWY!C2</f>
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="31">
         <v>120</v>
       </c>
@@ -24036,12 +24076,20 @@
       <c r="C5" s="33" t="s">
         <v>9</v>
       </c>
+      <c r="D5">
+        <f>$D4+A5</f>
+        <v>440</v>
+      </c>
       <c r="E5">
-        <f>A4+A3+A5+t_to_RWY!B3</f>
+        <f>$D5+t_to_RWY!B3</f>
         <v>1620</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <f>$D5+t_to_RWY!C3</f>
+        <v>940</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="31">
         <v>180</v>
       </c>
@@ -24051,12 +24099,20 @@
       <c r="C6" s="33" t="s">
         <v>10</v>
       </c>
+      <c r="D6">
+        <f>$D5+$A6</f>
+        <v>620</v>
+      </c>
       <c r="E6">
-        <f>A5+A4+A3+A6+t_to_RWY!B2</f>
+        <f>$D6+t_to_RWY!B2</f>
         <v>1320</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <f>$D6+t_to_RWY!C2</f>
+        <v>1660</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="31">
         <v>200</v>
       </c>
@@ -24066,12 +24122,20 @@
       <c r="C7" s="33" t="s">
         <v>9</v>
       </c>
+      <c r="D7">
+        <f t="shared" ref="D7:D11" si="0">$D6+$A7</f>
+        <v>820</v>
+      </c>
       <c r="E7">
-        <f>A7+A6+A5+A4+A3+t_to_RWY!B3</f>
+        <f>$D7+t_to_RWY!B3</f>
         <v>2000</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <f>$D7+t_to_RWY!C3</f>
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="31">
         <v>80</v>
       </c>
@@ -24081,12 +24145,20 @@
       <c r="C8" s="33" t="s">
         <v>10</v>
       </c>
+      <c r="D8">
+        <f t="shared" ref="D8:D11" si="1">$D7+A8</f>
+        <v>900</v>
+      </c>
       <c r="E8">
-        <f>A8+A7+A6+A5+A4+A3+t_to_RWY!B2</f>
+        <f>$D8+t_to_RWY!B2</f>
         <v>1600</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <f>$D8+t_to_RWY!C2</f>
+        <v>1940</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="31">
         <v>100</v>
       </c>
@@ -24096,12 +24168,20 @@
       <c r="C9" s="33" t="s">
         <v>10</v>
       </c>
+      <c r="D9">
+        <f t="shared" ref="D9:D11" si="2">$D8+$A9</f>
+        <v>1000</v>
+      </c>
       <c r="E9">
-        <f>A9+A8+A7+A6+A5+A4+A3+t_to_RWY!B4</f>
+        <f>$D9+t_to_RWY!B4</f>
         <v>1640</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <f>$D9+t_to_RWY!C4</f>
+        <v>2180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="31">
         <v>240</v>
       </c>
@@ -24111,12 +24191,20 @@
       <c r="C10" s="33" t="s">
         <v>9</v>
       </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>1240</v>
+      </c>
       <c r="E10">
-        <f>A9+A8+A7+A10+A6+A5+A4+A3+t_to_RWY!B2</f>
+        <f>$D10+t_to_RWY!B2</f>
         <v>1940</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F10">
+        <f>$D10+t_to_RWY!C2</f>
+        <v>2280</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="34">
         <v>80</v>
       </c>
@@ -24126,9 +24214,17 @@
       <c r="C11" s="36" t="s">
         <v>9</v>
       </c>
+      <c r="D11">
+        <f t="shared" ref="D11" si="3">$D10+A11</f>
+        <v>1320</v>
+      </c>
       <c r="E11">
-        <f>A10+A9+A8+A7+A6+A5+A4+A3+A11</f>
-        <v>1320</v>
+        <f>$D11+t_to_RWY!B3</f>
+        <v>2500</v>
+      </c>
+      <c r="F11">
+        <f>$D11+t_to_RWY!C3</f>
+        <v>1820</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Begonnen met Matlab files aan te passen voor scenarios
</commit_message>
<xml_diff>
--- a/runway-allocation - Correct/Full_Tables.xlsx
+++ b/runway-allocation - Correct/Full_Tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luka\Documents\runway-allocation\runway-allocation - Correct\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hofma\Documents\runway-allocation\runway-allocation - Correct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D46BCCA-02A3-4C73-987A-47B6D0E3AD5C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522E7808-6948-4D26-B4D7-30FE5FD45E53}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="R06_Arr_M" sheetId="2" r:id="rId1"/>
@@ -1480,8 +1480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6572479F-AFDE-4940-94F1-052247087792}">
   <dimension ref="A1:T281"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:P141"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11253,8 +11253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F2A5A1-E880-4844-A90B-E2D712D9D7B7}">
   <dimension ref="A1:Z281"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" topLeftCell="D128" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23964,8 +23964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD6EA91-B2D9-460A-B72F-58023DD02AD7}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24123,7 +24123,7 @@
         <v>9</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D11" si="0">$D6+$A7</f>
+        <f t="shared" ref="D7" si="0">$D6+$A7</f>
         <v>820</v>
       </c>
       <c r="E7">
@@ -24146,7 +24146,7 @@
         <v>10</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:D11" si="1">$D7+A8</f>
+        <f t="shared" ref="D8" si="1">$D7+A8</f>
         <v>900</v>
       </c>
       <c r="E8">
@@ -24169,7 +24169,7 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:D11" si="2">$D8+$A9</f>
+        <f t="shared" ref="D9:D10" si="2">$D8+$A9</f>
         <v>1000</v>
       </c>
       <c r="E9">

</xml_diff>

<commit_message>
Matlab klaar voor beide scenario's
</commit_message>
<xml_diff>
--- a/runway-allocation - Correct/Full_Tables.xlsx
+++ b/runway-allocation - Correct/Full_Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hofma\Documents\runway-allocation\runway-allocation - Correct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522E7808-6948-4D26-B4D7-30FE5FD45E53}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D39D6FB-E324-4EE9-A1F8-73406D11DBA5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="R06_Arr_M" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="29">
   <si>
     <t>Nr</t>
   </si>
@@ -11253,8 +11253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44F2A5A1-E880-4844-A90B-E2D712D9D7B7}">
   <dimension ref="A1:Z281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D128" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection sqref="A1:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23962,10 +23962,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD6EA91-B2D9-460A-B72F-58023DD02AD7}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24077,7 +24077,7 @@
         <v>9</v>
       </c>
       <c r="D5">
-        <f>$D4+A5</f>
+        <f t="shared" ref="D5:D11" si="0">$D4+$A5</f>
         <v>440</v>
       </c>
       <c r="E5">
@@ -24100,7 +24100,7 @@
         <v>10</v>
       </c>
       <c r="D6">
-        <f>$D5+$A6</f>
+        <f t="shared" si="0"/>
         <v>620</v>
       </c>
       <c r="E6">
@@ -24123,7 +24123,7 @@
         <v>9</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7" si="0">$D6+$A7</f>
+        <f t="shared" si="0"/>
         <v>820</v>
       </c>
       <c r="E7">
@@ -24146,7 +24146,7 @@
         <v>10</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8" si="1">$D7+A8</f>
+        <f t="shared" si="0"/>
         <v>900</v>
       </c>
       <c r="E8">
@@ -24169,7 +24169,7 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:D10" si="2">$D8+$A9</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="E9">
@@ -24192,7 +24192,7 @@
         <v>9</v>
       </c>
       <c r="D10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>1240</v>
       </c>
       <c r="E10">
@@ -24215,7 +24215,7 @@
         <v>9</v>
       </c>
       <c r="D11">
-        <f t="shared" ref="D11" si="3">$D10+A11</f>
+        <f t="shared" si="0"/>
         <v>1320</v>
       </c>
       <c r="E11">
@@ -24224,6 +24224,545 @@
       </c>
       <c r="F11">
         <f>$D11+t_to_RWY!C3</f>
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="28">
+        <v>220</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <f>t_to_RWY!B4</f>
+        <v>640</v>
+      </c>
+      <c r="F16">
+        <f>t_to_RWY!C4</f>
+        <v>1180</v>
+      </c>
+      <c r="H16" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16">
+        <f>MIN(E16:F25)</f>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="31">
+        <v>180</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17">
+        <f>$A17</f>
+        <v>180</v>
+      </c>
+      <c r="E17">
+        <f>$D17+t_to_RWY!$B$4</f>
+        <v>820</v>
+      </c>
+      <c r="F17">
+        <f>$D17+t_to_RWY!$C$4</f>
+        <v>1360</v>
+      </c>
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17">
+        <f>MAX(E16:F25)</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="31">
+        <v>140</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <f>$D17+$A18</f>
+        <v>320</v>
+      </c>
+      <c r="E18">
+        <f>$D18+t_to_RWY!$B$4</f>
+        <v>960</v>
+      </c>
+      <c r="F18">
+        <f>$D18+t_to_RWY!$C$4</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="31">
+        <v>120</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ref="D19:D25" si="1">$D18+$A19</f>
+        <v>440</v>
+      </c>
+      <c r="E19">
+        <f>$D19+t_to_RWY!$B$4</f>
+        <v>1080</v>
+      </c>
+      <c r="F19">
+        <f>$D19+t_to_RWY!$C$4</f>
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="31">
+        <v>180</v>
+      </c>
+      <c r="B20" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>620</v>
+      </c>
+      <c r="E20">
+        <f>$D20+t_to_RWY!$B$4</f>
+        <v>1260</v>
+      </c>
+      <c r="F20">
+        <f>$D20+t_to_RWY!$C$4</f>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="31">
+        <v>200</v>
+      </c>
+      <c r="B21" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>820</v>
+      </c>
+      <c r="E21">
+        <f>$D21+t_to_RWY!$B$4</f>
+        <v>1460</v>
+      </c>
+      <c r="F21">
+        <f>$D21+t_to_RWY!$C$4</f>
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="31">
+        <v>80</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>900</v>
+      </c>
+      <c r="E22">
+        <f>$D22+t_to_RWY!$B$4</f>
+        <v>1540</v>
+      </c>
+      <c r="F22">
+        <f>$D22+t_to_RWY!$C$4</f>
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="31">
+        <v>100</v>
+      </c>
+      <c r="B23" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="E23">
+        <f>$D23+t_to_RWY!$B$4</f>
+        <v>1640</v>
+      </c>
+      <c r="F23">
+        <f>$D23+t_to_RWY!$C$4</f>
+        <v>2180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="31">
+        <v>240</v>
+      </c>
+      <c r="B24" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>1240</v>
+      </c>
+      <c r="E24">
+        <f>$D24+t_to_RWY!$B$4</f>
+        <v>1880</v>
+      </c>
+      <c r="F24">
+        <f>$D24+t_to_RWY!$C$4</f>
+        <v>2420</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="34">
+        <v>80</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>1320</v>
+      </c>
+      <c r="E25">
+        <f>$D25+t_to_RWY!$B$4</f>
+        <v>1960</v>
+      </c>
+      <c r="F25">
+        <f>$D25+t_to_RWY!$C$4</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="28">
+        <v>220</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30">
+        <f>t_to_RWY!B3</f>
+        <v>1180</v>
+      </c>
+      <c r="F30">
+        <f>t_to_RWY!C3</f>
+        <v>500</v>
+      </c>
+      <c r="H30" t="s">
+        <v>27</v>
+      </c>
+      <c r="I30">
+        <f>MIN(E30:F39)</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="31">
+        <v>180</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31">
+        <v>180</v>
+      </c>
+      <c r="E31">
+        <f>$D31+t_to_RWY!$B$3</f>
+        <v>1360</v>
+      </c>
+      <c r="F31">
+        <f>$D31+t_to_RWY!$C$3</f>
+        <v>680</v>
+      </c>
+      <c r="H31" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31">
+        <f>MAX(E30:F39)</f>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="31">
+        <v>140</v>
+      </c>
+      <c r="B32" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <f>$D31+$A32</f>
+        <v>320</v>
+      </c>
+      <c r="E32">
+        <f>$D32+t_to_RWY!$B$3</f>
+        <v>1500</v>
+      </c>
+      <c r="F32">
+        <f>$D32+t_to_RWY!$C$3</f>
+        <v>820</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="31">
+        <v>120</v>
+      </c>
+      <c r="B33" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33">
+        <f t="shared" ref="D33:D39" si="2">$D32+$A33</f>
+        <v>440</v>
+      </c>
+      <c r="E33">
+        <f>$D33+t_to_RWY!$B$3</f>
+        <v>1620</v>
+      </c>
+      <c r="F33">
+        <f>$D33+t_to_RWY!$C$3</f>
+        <v>940</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="31">
+        <v>180</v>
+      </c>
+      <c r="B34" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="2"/>
+        <v>620</v>
+      </c>
+      <c r="E34">
+        <f>$D34+t_to_RWY!$B$3</f>
+        <v>1800</v>
+      </c>
+      <c r="F34">
+        <f>$D34+t_to_RWY!$C$3</f>
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="31">
+        <v>200</v>
+      </c>
+      <c r="B35" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="2"/>
+        <v>820</v>
+      </c>
+      <c r="E35">
+        <f>$D35+t_to_RWY!$B$3</f>
+        <v>2000</v>
+      </c>
+      <c r="F35">
+        <f>$D35+t_to_RWY!$C$3</f>
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="31">
+        <v>80</v>
+      </c>
+      <c r="B36" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="2"/>
+        <v>900</v>
+      </c>
+      <c r="E36">
+        <f>$D36+t_to_RWY!$B$3</f>
+        <v>2080</v>
+      </c>
+      <c r="F36">
+        <f>$D36+t_to_RWY!$C$3</f>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="31">
+        <v>100</v>
+      </c>
+      <c r="B37" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="2"/>
+        <v>1000</v>
+      </c>
+      <c r="E37">
+        <f>$D37+t_to_RWY!$B$3</f>
+        <v>2180</v>
+      </c>
+      <c r="F37">
+        <f>$D37+t_to_RWY!$C$3</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="31">
+        <v>240</v>
+      </c>
+      <c r="B38" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="2"/>
+        <v>1240</v>
+      </c>
+      <c r="E38">
+        <f>$D38+t_to_RWY!$B$3</f>
+        <v>2420</v>
+      </c>
+      <c r="F38">
+        <f>$D38+t_to_RWY!$C$3</f>
+        <v>1740</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="34">
+        <v>80</v>
+      </c>
+      <c r="B39" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="2"/>
+        <v>1320</v>
+      </c>
+      <c r="E39">
+        <f>$D39+t_to_RWY!$B$3</f>
+        <v>2500</v>
+      </c>
+      <c r="F39">
+        <f>$D39+t_to_RWY!$C$3</f>
         <v>1820</v>
       </c>
     </row>

</xml_diff>